<commit_message>
sql database and queries
</commit_message>
<xml_diff>
--- a/price_tables.xlsx
+++ b/price_tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\price_databse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\projects\price_databse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8561B2B3-C11A-40FD-ACF5-85838C583ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F2DB6E-DD9E-4939-B190-7DC73E3C8CBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="675" windowWidth="24000" windowHeight="16830" xr2:uid="{6F190CA3-FE5A-4655-9EB8-91AC85BCDFEC}"/>
+    <workbookView xWindow="21720" yWindow="1575" windowWidth="14250" windowHeight="12765" activeTab="1" xr2:uid="{6F190CA3-FE5A-4655-9EB8-91AC85BCDFEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="116">
   <si>
     <t>pvc_type_id</t>
   </si>
@@ -362,6 +362,24 @@
   </si>
   <si>
     <t>Single Door Y</t>
+  </si>
+  <si>
+    <t>Type 1400</t>
+  </si>
+  <si>
+    <t>Type 1100</t>
+  </si>
+  <si>
+    <t>Type 700</t>
+  </si>
+  <si>
+    <t>Type 400</t>
+  </si>
+  <si>
+    <t>Type 250 SS</t>
+  </si>
+  <si>
+    <t>Type 400 SS</t>
   </si>
 </sst>
 </file>
@@ -414,7 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -432,6 +450,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -749,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE05D96-DD6A-442B-BADE-CCDCA32DB199}">
   <dimension ref="A1:O174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G133" workbookViewId="0">
-      <selection activeCell="I148" sqref="I148"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,8 +850,8 @@
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" s="5">
-        <v>1400</v>
+      <c r="I3" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="K3" s="1">
         <v>1</v>
@@ -869,8 +888,8 @@
       <c r="H4">
         <v>2</v>
       </c>
-      <c r="I4" s="5">
-        <v>1100</v>
+      <c r="I4" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="K4" s="1">
         <v>2</v>
@@ -907,8 +926,8 @@
       <c r="H5">
         <v>3</v>
       </c>
-      <c r="I5" s="5">
-        <v>700</v>
+      <c r="I5" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="K5" s="1">
         <v>3</v>
@@ -945,8 +964,8 @@
       <c r="H6">
         <v>4</v>
       </c>
-      <c r="I6" s="5">
-        <v>400</v>
+      <c r="I6" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="K6" s="1">
         <v>4</v>
@@ -984,7 +1003,7 @@
         <v>5</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="K7" s="1">
         <v>5</v>
@@ -1022,7 +1041,7 @@
         <v>6</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="K8" s="1">
         <v>6</v>
@@ -4250,8 +4269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D206C3-9B0F-4080-806E-15E489CAE7D2}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4287,7 +4306,7 @@
         <v>93</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -4321,7 +4340,7 @@
       <c r="J2" s="2">
         <v>1</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="7">
         <v>410</v>
       </c>
     </row>
@@ -4350,7 +4369,7 @@
       <c r="J3" s="1">
         <v>2</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="7">
         <v>970</v>
       </c>
     </row>
@@ -4379,7 +4398,7 @@
       <c r="J4" s="1">
         <v>3</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="7">
         <v>1800</v>
       </c>
     </row>
@@ -4408,7 +4427,7 @@
       <c r="J5" s="1">
         <v>4</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="7">
         <v>2580</v>
       </c>
     </row>
@@ -4437,7 +4456,7 @@
       <c r="J6" s="1">
         <v>5</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="7">
         <v>3640</v>
       </c>
     </row>
@@ -4466,7 +4485,7 @@
       <c r="J7" s="1">
         <v>6</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="7">
         <v>5870</v>
       </c>
     </row>
@@ -4495,7 +4514,7 @@
       <c r="J8" s="1">
         <v>7</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="7">
         <v>10330</v>
       </c>
     </row>
@@ -4524,7 +4543,7 @@
       <c r="J9" s="1">
         <v>8</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="7">
         <v>18090</v>
       </c>
     </row>
@@ -4553,7 +4572,7 @@
       <c r="J10" s="1">
         <v>9</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="7">
         <v>22980</v>
       </c>
     </row>
@@ -4582,7 +4601,7 @@
       <c r="J11" s="1">
         <v>3</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="7">
         <v>700</v>
       </c>
     </row>
@@ -4605,7 +4624,7 @@
       <c r="J12" s="1">
         <v>4</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="7">
         <v>1750</v>
       </c>
     </row>
@@ -4628,7 +4647,7 @@
       <c r="J13" s="1">
         <v>5</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="7">
         <v>2070</v>
       </c>
     </row>
@@ -4651,7 +4670,7 @@
       <c r="J14" s="1">
         <v>6</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="7">
         <v>3680</v>
       </c>
     </row>
@@ -4674,7 +4693,7 @@
       <c r="J15" s="1">
         <v>7</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="7">
         <v>7180</v>
       </c>
     </row>
@@ -4697,7 +4716,7 @@
       <c r="J16" s="1">
         <v>8</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="7">
         <v>11535</v>
       </c>
     </row>
@@ -4720,7 +4739,7 @@
       <c r="J17" s="1">
         <v>9</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="7">
         <v>15945</v>
       </c>
     </row>
@@ -4743,7 +4762,7 @@
       <c r="J18" s="1">
         <v>5</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="7">
         <v>1500</v>
       </c>
     </row>
@@ -4766,7 +4785,7 @@
       <c r="J19" s="1">
         <v>6</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="7">
         <v>2880</v>
       </c>
     </row>
@@ -4789,7 +4808,7 @@
       <c r="J20" s="1">
         <v>7</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="7">
         <v>4540</v>
       </c>
     </row>
@@ -4812,7 +4831,7 @@
       <c r="J21" s="1">
         <v>8</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="7">
         <v>7665</v>
       </c>
     </row>
@@ -4835,7 +4854,7 @@
       <c r="J22" s="1">
         <v>9</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="7">
         <v>7530</v>
       </c>
     </row>
@@ -4858,7 +4877,7 @@
       <c r="J23" s="2">
         <v>9</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="7">
         <v>4635</v>
       </c>
     </row>
@@ -4881,7 +4900,7 @@
       <c r="J24" s="2">
         <v>9</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K24" s="7">
         <v>7590</v>
       </c>
     </row>
@@ -4904,7 +4923,7 @@
       <c r="J25" s="2">
         <v>6</v>
       </c>
-      <c r="K25" s="4">
+      <c r="K25" s="7">
         <v>1070</v>
       </c>
     </row>
@@ -4927,7 +4946,7 @@
       <c r="J26" s="2">
         <v>9</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K26" s="7">
         <v>3015</v>
       </c>
     </row>
@@ -4950,7 +4969,7 @@
       <c r="J27" s="2">
         <v>9</v>
       </c>
-      <c r="K27" s="4">
+      <c r="K27" s="7">
         <v>3750</v>
       </c>
     </row>

</xml_diff>